<commit_message>
pesudocode and sprint backlog type corrected
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_1_SprintBacklog.xlsx
+++ b/TutorGroup_Deliverable_1_SprintBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1585A10-7D5F-F047-88B0-8FE8558683A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065D983-8527-3044-AC34-394F86912B61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="460" windowWidth="23860" windowHeight="12980" xr2:uid="{1DCDFF68-8BA1-1048-B1AC-C259A1B80F61}"/>
+    <workbookView xWindow="15640" yWindow="460" windowWidth="17680" windowHeight="15700" xr2:uid="{1DCDFF68-8BA1-1048-B1AC-C259A1B80F61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Number</t>
   </si>
@@ -57,9 +57,6 @@
     <t>As a student user I would like to be able to post listings so that I can find a tutor.</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>As a student user I need to have a customizable student profile so that I can add basic information about me and what my interests are.</t>
   </si>
   <si>
@@ -75,7 +72,7 @@
     <t>As a general user I would like to have a toolbar to access the various applications features.</t>
   </si>
   <si>
-    <t>M</t>
+    <t>F,T</t>
   </si>
 </sst>
 </file>
@@ -451,7 +448,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,11 +485,11 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
         <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -503,13 +500,13 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
         <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -520,13 +517,13 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -537,13 +534,13 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -554,13 +551,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
         <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -571,13 +568,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
       <c r="E7">
         <v>0</v>

</xml_diff>